<commit_message>
vault backup: 2024-11-08 12:32:55
</commit_message>
<xml_diff>
--- a/financial/backtesting/data.xlsx
+++ b/financial/backtesting/data.xlsx
@@ -502,2401 +502,2401 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>花旗環球</t>
+          <t>摩根大通</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.126</v>
+        <v>0.0388</v>
       </c>
       <c r="D2" t="n">
-        <v>591657.1</v>
+        <v>276639.1</v>
       </c>
       <c r="E2" t="n">
-        <v>54718.5</v>
+        <v>16066</v>
       </c>
       <c r="F2" t="n">
-        <v>536938.6</v>
+        <v>260573.1</v>
       </c>
       <c r="G2" t="n">
-        <v>-59963</v>
+        <v>-31381</v>
       </c>
       <c r="H2" t="n">
-        <v>22156</v>
+        <v>95966</v>
       </c>
       <c r="I2" t="n">
-        <v>82119</v>
+        <v>127347</v>
       </c>
       <c r="J2" t="n">
-        <v>57.2</v>
+        <v>55.9</v>
       </c>
       <c r="K2" t="n">
-        <v>55.2</v>
+        <v>55.8</v>
       </c>
       <c r="L2" t="n">
-        <v>57.7</v>
+        <v>56</v>
       </c>
       <c r="M2" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1590&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8440&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>台灣摩根士丹利</t>
+          <t>凱基-台北</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.0852</v>
+        <v>0.0221</v>
       </c>
       <c r="D3" t="n">
-        <v>488647</v>
+        <v>127792.9</v>
       </c>
       <c r="E3" t="n">
-        <v>220141.5</v>
+        <v>38108.2</v>
       </c>
       <c r="F3" t="n">
-        <v>268505.5</v>
+        <v>89684.8</v>
       </c>
       <c r="G3" t="n">
-        <v>-34512</v>
+        <v>-11246</v>
       </c>
       <c r="H3" t="n">
-        <v>69282</v>
+        <v>92895</v>
       </c>
       <c r="I3" t="n">
-        <v>103794</v>
+        <v>104142</v>
       </c>
       <c r="J3" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="K3" t="n">
         <v>55.3</v>
       </c>
-      <c r="K3" t="n">
-        <v>53.4</v>
-      </c>
       <c r="L3" t="n">
-        <v>56.5</v>
+        <v>55.7</v>
       </c>
       <c r="M3" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1470&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9268&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>摩根大通</t>
+          <t>美商高盛</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.0342</v>
+        <v>0.0336</v>
       </c>
       <c r="D4" t="n">
-        <v>243689.1</v>
+        <v>207552.1</v>
       </c>
       <c r="E4" t="n">
-        <v>16066</v>
+        <v>9220.6</v>
       </c>
       <c r="F4" t="n">
-        <v>227623.1</v>
+        <v>198331.5</v>
       </c>
       <c r="G4" t="n">
-        <v>-31381</v>
+        <v>-30121</v>
       </c>
       <c r="H4" t="n">
-        <v>95966</v>
+        <v>83812</v>
       </c>
       <c r="I4" t="n">
-        <v>127347</v>
+        <v>113934</v>
       </c>
       <c r="J4" t="n">
-        <v>55.9</v>
+        <v>54.2</v>
       </c>
       <c r="K4" t="n">
-        <v>55.8</v>
+        <v>54.2</v>
       </c>
       <c r="L4" t="n">
-        <v>56</v>
+        <v>54.3</v>
       </c>
       <c r="M4" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8440&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1480&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>國泰</t>
+          <t>台灣摩根士丹利</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.1222</v>
+        <v>0.0915</v>
       </c>
       <c r="D5" t="n">
-        <v>227908.9</v>
+        <v>524884.6</v>
       </c>
       <c r="E5" t="n">
-        <v>17942.9</v>
+        <v>220141.5</v>
       </c>
       <c r="F5" t="n">
-        <v>209966</v>
+        <v>304743.1</v>
       </c>
       <c r="G5" t="n">
-        <v>-24593</v>
+        <v>-34512</v>
       </c>
       <c r="H5" t="n">
-        <v>8205</v>
+        <v>69282</v>
       </c>
       <c r="I5" t="n">
-        <v>32798</v>
+        <v>103794</v>
       </c>
       <c r="J5" t="n">
-        <v>56.9</v>
+        <v>55.3</v>
       </c>
       <c r="K5" t="n">
-        <v>55.1</v>
+        <v>53.4</v>
       </c>
       <c r="L5" t="n">
-        <v>57.3</v>
+        <v>56.5</v>
       </c>
       <c r="M5" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8880&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1470&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>臺銀證券</t>
+          <t>元大</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.06809999999999999</v>
+        <v>0.034</v>
       </c>
       <c r="D6" t="n">
-        <v>194337.2</v>
+        <v>133084</v>
       </c>
       <c r="E6" t="n">
-        <v>-2960.8</v>
+        <v>-6072.8</v>
       </c>
       <c r="F6" t="n">
-        <v>197298</v>
+        <v>139156.7</v>
       </c>
       <c r="G6" t="n">
-        <v>-51088</v>
+        <v>-18512</v>
       </c>
       <c r="H6" t="n">
-        <v>3091</v>
+        <v>52393</v>
       </c>
       <c r="I6" t="n">
-        <v>54180</v>
+        <v>70906</v>
       </c>
       <c r="J6" t="n">
-        <v>52.7</v>
+        <v>55.3</v>
       </c>
       <c r="K6" t="n">
-        <v>53.6</v>
+        <v>55.3</v>
       </c>
       <c r="L6" t="n">
-        <v>52.6</v>
+        <v>55.2</v>
       </c>
       <c r="M6" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1040&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9800&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>美商高盛</t>
+          <t>花旗環球</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.0285</v>
+        <v>0.1394</v>
       </c>
       <c r="D7" t="n">
-        <v>175924</v>
+        <v>654618.2</v>
       </c>
       <c r="E7" t="n">
-        <v>9220.6</v>
+        <v>54718.5</v>
       </c>
       <c r="F7" t="n">
-        <v>166703.4</v>
+        <v>599899.7</v>
       </c>
       <c r="G7" t="n">
-        <v>-30121</v>
+        <v>-59963</v>
       </c>
       <c r="H7" t="n">
-        <v>83812</v>
+        <v>22156</v>
       </c>
       <c r="I7" t="n">
-        <v>113934</v>
+        <v>82119</v>
       </c>
       <c r="J7" t="n">
-        <v>54.2</v>
+        <v>57.2</v>
       </c>
       <c r="K7" t="n">
-        <v>54.2</v>
+        <v>55.2</v>
       </c>
       <c r="L7" t="n">
-        <v>54.3</v>
+        <v>57.7</v>
       </c>
       <c r="M7" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1480&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1590&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>凱基-台北</t>
+          <t>港商野村</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.0201</v>
+        <v>0.019</v>
       </c>
       <c r="D8" t="n">
-        <v>115983.6</v>
+        <v>17508</v>
       </c>
       <c r="E8" t="n">
-        <v>38108.2</v>
+        <v>5669.2</v>
       </c>
       <c r="F8" t="n">
-        <v>77875.39999999999</v>
+        <v>11838.8</v>
       </c>
       <c r="G8" t="n">
-        <v>-11246</v>
+        <v>-2667</v>
       </c>
       <c r="H8" t="n">
-        <v>92895</v>
+        <v>15048</v>
       </c>
       <c r="I8" t="n">
-        <v>104142</v>
+        <v>17716</v>
       </c>
       <c r="J8" t="n">
-        <v>55.5</v>
+        <v>52</v>
       </c>
       <c r="K8" t="n">
-        <v>55.3</v>
+        <v>51.8</v>
       </c>
       <c r="L8" t="n">
-        <v>55.7</v>
+        <v>52.1</v>
       </c>
       <c r="M8" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9268&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1560&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>元大</t>
+          <t>元富</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.029</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>113645.3</v>
+        <v>5475.1</v>
       </c>
       <c r="E9" t="n">
-        <v>-6072.8</v>
+        <v>-10938.1</v>
       </c>
       <c r="F9" t="n">
-        <v>119718.1</v>
+        <v>16413.2</v>
       </c>
       <c r="G9" t="n">
-        <v>-18512</v>
+        <v>-2252</v>
       </c>
       <c r="H9" t="n">
-        <v>52393</v>
+        <v>11813</v>
       </c>
       <c r="I9" t="n">
-        <v>70906</v>
+        <v>14066</v>
       </c>
       <c r="J9" t="n">
-        <v>55.3</v>
+        <v>55.4</v>
       </c>
       <c r="K9" t="n">
-        <v>55.3</v>
+        <v>55.9</v>
       </c>
       <c r="L9" t="n">
-        <v>55.2</v>
+        <v>55</v>
       </c>
       <c r="M9" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9800&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=5920&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>富邦</t>
+          <t>國泰</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.1049</v>
+        <v>0.1361</v>
       </c>
       <c r="D10" t="n">
-        <v>104625.3</v>
+        <v>253731.5</v>
       </c>
       <c r="E10" t="n">
-        <v>16313</v>
+        <v>17942.9</v>
       </c>
       <c r="F10" t="n">
-        <v>88312.39999999999</v>
+        <v>235788.6</v>
       </c>
       <c r="G10" t="n">
-        <v>-9490</v>
+        <v>-24593</v>
       </c>
       <c r="H10" t="n">
-        <v>7880</v>
+        <v>8205</v>
       </c>
       <c r="I10" t="n">
-        <v>17371</v>
+        <v>32798</v>
       </c>
       <c r="J10" t="n">
-        <v>57.4</v>
+        <v>56.9</v>
       </c>
       <c r="K10" t="n">
-        <v>56</v>
+        <v>55.1</v>
       </c>
       <c r="L10" t="n">
-        <v>58.1</v>
+        <v>57.3</v>
       </c>
       <c r="M10" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9600&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8880&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>台灣匯立</t>
+          <t>富邦</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.1445</v>
+        <v>0.1149</v>
       </c>
       <c r="D11" t="n">
-        <v>65499.5</v>
+        <v>114590.9</v>
       </c>
       <c r="E11" t="n">
-        <v>55739.1</v>
+        <v>16313</v>
       </c>
       <c r="F11" t="n">
-        <v>9760.4</v>
+        <v>98277.89999999999</v>
       </c>
       <c r="G11" t="n">
-        <v>-752</v>
+        <v>-9490</v>
       </c>
       <c r="H11" t="n">
-        <v>7069</v>
+        <v>7880</v>
       </c>
       <c r="I11" t="n">
-        <v>7822</v>
+        <v>17371</v>
       </c>
       <c r="J11" t="n">
-        <v>58</v>
+        <v>57.4</v>
       </c>
       <c r="K11" t="n">
-        <v>53.8</v>
+        <v>56</v>
       </c>
       <c r="L11" t="n">
-        <v>61.7</v>
+        <v>58.1</v>
       </c>
       <c r="M11" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1380&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9600&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>兆豐</t>
+          <t>凱基</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.06509999999999999</v>
+        <v>0.0155</v>
       </c>
       <c r="D12" t="n">
-        <v>51627.4</v>
+        <v>6563.4</v>
       </c>
       <c r="E12" t="n">
-        <v>1688.7</v>
+        <v>3401.9</v>
       </c>
       <c r="F12" t="n">
-        <v>49938.7</v>
+        <v>3161.5</v>
       </c>
       <c r="G12" t="n">
-        <v>-9255</v>
+        <v>-535</v>
       </c>
       <c r="H12" t="n">
-        <v>5408</v>
+        <v>7419</v>
       </c>
       <c r="I12" t="n">
-        <v>14664</v>
+        <v>7954</v>
       </c>
       <c r="J12" t="n">
-        <v>54.1</v>
+        <v>53.4</v>
       </c>
       <c r="K12" t="n">
-        <v>53.8</v>
+        <v>53.2</v>
       </c>
       <c r="L12" t="n">
-        <v>54.1</v>
+        <v>53.6</v>
       </c>
       <c r="M12" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=7000&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9200&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>港商麥格理</t>
+          <t>台灣匯立</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.09880000000000001</v>
+        <v>0.1462</v>
       </c>
       <c r="D13" t="n">
-        <v>49826.1</v>
+        <v>66290.10000000001</v>
       </c>
       <c r="E13" t="n">
-        <v>12107.2</v>
+        <v>55739.1</v>
       </c>
       <c r="F13" t="n">
-        <v>37718.9</v>
+        <v>10551.1</v>
       </c>
       <c r="G13" t="n">
-        <v>-3797</v>
+        <v>-752</v>
       </c>
       <c r="H13" t="n">
-        <v>4930</v>
+        <v>7069</v>
       </c>
       <c r="I13" t="n">
-        <v>8728</v>
+        <v>7822</v>
       </c>
       <c r="J13" t="n">
-        <v>57.8</v>
+        <v>58</v>
       </c>
       <c r="K13" t="n">
-        <v>56.2</v>
+        <v>53.8</v>
       </c>
       <c r="L13" t="n">
-        <v>58.7</v>
+        <v>61.7</v>
       </c>
       <c r="M13" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1360&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1380&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>彰銀</t>
+          <t>華南永昌</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.09810000000000001</v>
+        <v>0.0021</v>
       </c>
       <c r="D14" t="n">
-        <v>44394.3</v>
+        <v>775.5</v>
       </c>
       <c r="E14" t="n">
-        <v>-1319.2</v>
+        <v>385.2</v>
       </c>
       <c r="F14" t="n">
-        <v>45713.5</v>
+        <v>390.3</v>
       </c>
       <c r="G14" t="n">
-        <v>-7432</v>
+        <v>-55</v>
       </c>
       <c r="H14" t="n">
-        <v>790</v>
+        <v>6797</v>
       </c>
       <c r="I14" t="n">
-        <v>8222</v>
+        <v>6853</v>
       </c>
       <c r="J14" t="n">
-        <v>55</v>
+        <v>54.6</v>
       </c>
       <c r="K14" t="n">
-        <v>56.6</v>
+        <v>54.6</v>
       </c>
       <c r="L14" t="n">
-        <v>54.9</v>
+        <v>54.7</v>
       </c>
       <c r="M14" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1230&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9300&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>香港上海匯豐</t>
+          <t>玉山</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.1302</v>
+        <v>0.0292</v>
       </c>
       <c r="D15" t="n">
-        <v>40061.6</v>
+        <v>10502.4</v>
       </c>
       <c r="E15" t="n">
-        <v>31233</v>
+        <v>14056.5</v>
       </c>
       <c r="F15" t="n">
-        <v>8828.6</v>
+        <v>-3554.1</v>
       </c>
       <c r="G15" t="n">
-        <v>-792</v>
+        <v>490</v>
       </c>
       <c r="H15" t="n">
-        <v>4628</v>
+        <v>6424</v>
       </c>
       <c r="I15" t="n">
-        <v>5421</v>
+        <v>5933</v>
       </c>
       <c r="J15" t="n">
-        <v>56.8</v>
+        <v>56.1</v>
       </c>
       <c r="K15" t="n">
-        <v>53.1</v>
+        <v>54.9</v>
       </c>
       <c r="L15" t="n">
-        <v>59.9</v>
+        <v>57.3</v>
       </c>
       <c r="M15" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8960&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8840&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>大和國泰</t>
+          <t>富邦-台北</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.0771</v>
+        <v>0.0229</v>
       </c>
       <c r="D16" t="n">
-        <v>33852.7</v>
+        <v>7540.8</v>
       </c>
       <c r="E16" t="n">
-        <v>-3485.6</v>
+        <v>3645.8</v>
       </c>
       <c r="F16" t="n">
-        <v>37338.3</v>
+        <v>3895</v>
       </c>
       <c r="G16" t="n">
-        <v>-6806</v>
+        <v>-536</v>
       </c>
       <c r="H16" t="n">
-        <v>1234</v>
+        <v>5491</v>
       </c>
       <c r="I16" t="n">
-        <v>8041</v>
+        <v>6028</v>
       </c>
       <c r="J16" t="n">
         <v>54.6</v>
       </c>
       <c r="K16" t="n">
-        <v>57.1</v>
+        <v>54.3</v>
       </c>
       <c r="L16" t="n">
-        <v>54.2</v>
+        <v>55</v>
       </c>
       <c r="M16" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8890&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9623&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>國票-敦北法人</t>
+          <t>兆豐</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.0341</v>
+        <v>0.0774</v>
       </c>
       <c r="D17" t="n">
-        <v>15347.9</v>
+        <v>61346.2</v>
       </c>
       <c r="E17" t="n">
-        <v>-4117.9</v>
+        <v>1688.7</v>
       </c>
       <c r="F17" t="n">
-        <v>19465.9</v>
+        <v>59657.5</v>
       </c>
       <c r="G17" t="n">
-        <v>-6581</v>
+        <v>-9255</v>
       </c>
       <c r="H17" t="n">
-        <v>2051</v>
+        <v>5408</v>
       </c>
       <c r="I17" t="n">
-        <v>8633</v>
+        <v>14664</v>
       </c>
       <c r="J17" t="n">
-        <v>52.1</v>
+        <v>54.1</v>
       </c>
       <c r="K17" t="n">
-        <v>53.7</v>
+        <v>53.8</v>
       </c>
       <c r="L17" t="n">
-        <v>51.7</v>
+        <v>54.1</v>
       </c>
       <c r="M17" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=779c&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=7000&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>港商野村</t>
+          <t>元大-士林</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.016</v>
+        <v>0.0157</v>
       </c>
       <c r="D18" t="n">
-        <v>14706.6</v>
+        <v>4475.9</v>
       </c>
       <c r="E18" t="n">
-        <v>5669.2</v>
+        <v>12051.6</v>
       </c>
       <c r="F18" t="n">
-        <v>9037.5</v>
+        <v>-7575.7</v>
       </c>
       <c r="G18" t="n">
-        <v>-2667</v>
+        <v>1877</v>
       </c>
       <c r="H18" t="n">
-        <v>15048</v>
+        <v>5375</v>
       </c>
       <c r="I18" t="n">
-        <v>17716</v>
+        <v>3498</v>
       </c>
       <c r="J18" t="n">
-        <v>52</v>
+        <v>53.1</v>
       </c>
       <c r="K18" t="n">
-        <v>51.8</v>
+        <v>51.7</v>
       </c>
       <c r="L18" t="n">
-        <v>52.1</v>
+        <v>55.2</v>
       </c>
       <c r="M18" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1560&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=981j&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>玉山</t>
+          <t>港商麥格理</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.0306</v>
+        <v>0.1067</v>
       </c>
       <c r="D19" t="n">
-        <v>11017.9</v>
+        <v>53814</v>
       </c>
       <c r="E19" t="n">
-        <v>14056.5</v>
+        <v>12107.2</v>
       </c>
       <c r="F19" t="n">
-        <v>-3038.6</v>
+        <v>41706.8</v>
       </c>
       <c r="G19" t="n">
-        <v>490</v>
+        <v>-3797</v>
       </c>
       <c r="H19" t="n">
-        <v>6424</v>
+        <v>4930</v>
       </c>
       <c r="I19" t="n">
-        <v>5933</v>
+        <v>8728</v>
       </c>
       <c r="J19" t="n">
-        <v>56.1</v>
+        <v>57.8</v>
       </c>
       <c r="K19" t="n">
-        <v>54.9</v>
+        <v>56.2</v>
       </c>
       <c r="L19" t="n">
-        <v>57.3</v>
+        <v>58.7</v>
       </c>
       <c r="M19" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8840&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1360&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>新加坡商瑞銀</t>
+          <t>香港上海匯豐</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.0018</v>
+        <v>0.1329</v>
       </c>
       <c r="D20" t="n">
-        <v>10542.1</v>
+        <v>40894.3</v>
       </c>
       <c r="E20" t="n">
-        <v>66976.8</v>
+        <v>31233</v>
       </c>
       <c r="F20" t="n">
-        <v>-56434.7</v>
+        <v>9661.299999999999</v>
       </c>
       <c r="G20" t="n">
-        <v>9831</v>
+        <v>-792</v>
       </c>
       <c r="H20" t="n">
-        <v>108000</v>
+        <v>4628</v>
       </c>
       <c r="I20" t="n">
-        <v>98169</v>
+        <v>5421</v>
       </c>
       <c r="J20" t="n">
-        <v>54.8</v>
+        <v>56.8</v>
       </c>
       <c r="K20" t="n">
-        <v>54.5</v>
+        <v>53.1</v>
       </c>
       <c r="L20" t="n">
-        <v>55.2</v>
+        <v>59.9</v>
       </c>
       <c r="M20" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1650&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8960&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>第一金</t>
+          <t>中國信託</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.0446</v>
+        <v>0.0038</v>
       </c>
       <c r="D21" t="n">
-        <v>9204.5</v>
+        <v>1154.8</v>
       </c>
       <c r="E21" t="n">
-        <v>-3129.4</v>
+        <v>-7555.8</v>
       </c>
       <c r="F21" t="n">
-        <v>12333.9</v>
+        <v>8710.5</v>
       </c>
       <c r="G21" t="n">
-        <v>-2703</v>
+        <v>-1456</v>
       </c>
       <c r="H21" t="n">
-        <v>1122</v>
+        <v>4117</v>
       </c>
       <c r="I21" t="n">
-        <v>3825</v>
+        <v>5574</v>
       </c>
       <c r="J21" t="n">
-        <v>53.9</v>
+        <v>54.5</v>
       </c>
       <c r="K21" t="n">
-        <v>56.1</v>
+        <v>55.5</v>
       </c>
       <c r="L21" t="n">
-        <v>53.3</v>
+        <v>53.7</v>
       </c>
       <c r="M21" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=5380&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=6160&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>華南永昌-嘉義</t>
+          <t>國票</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.0521</v>
+        <v>0.008699999999999999</v>
       </c>
       <c r="D22" t="n">
-        <v>8252.299999999999</v>
+        <v>1875.8</v>
       </c>
       <c r="E22" t="n">
-        <v>-2227.5</v>
+        <v>-123.7</v>
       </c>
       <c r="F22" t="n">
-        <v>10479.8</v>
+        <v>1999.5</v>
       </c>
       <c r="G22" t="n">
-        <v>-2357</v>
+        <v>-228</v>
       </c>
       <c r="H22" t="n">
-        <v>587</v>
+        <v>3581</v>
       </c>
       <c r="I22" t="n">
-        <v>2945</v>
+        <v>3810</v>
       </c>
       <c r="J22" t="n">
-        <v>53.8</v>
+        <v>56.4</v>
       </c>
       <c r="K22" t="n">
-        <v>57</v>
+        <v>56.5</v>
       </c>
       <c r="L22" t="n">
-        <v>53.2</v>
+        <v>56.4</v>
       </c>
       <c r="M22" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9314&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=7790&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>台灣企銀</t>
+          <t>臺銀證券</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.05139999999999999</v>
+        <v>0.08689999999999999</v>
       </c>
       <c r="D23" t="n">
-        <v>7462.2</v>
+        <v>247980.6</v>
       </c>
       <c r="E23" t="n">
-        <v>1257.9</v>
+        <v>-2960.8</v>
       </c>
       <c r="F23" t="n">
-        <v>6204.3</v>
+        <v>250941.4</v>
       </c>
       <c r="G23" t="n">
-        <v>-1138</v>
+        <v>-51088</v>
       </c>
       <c r="H23" t="n">
-        <v>1553</v>
+        <v>3091</v>
       </c>
       <c r="I23" t="n">
-        <v>2692</v>
+        <v>54180</v>
       </c>
       <c r="J23" t="n">
-        <v>53.9</v>
+        <v>52.7</v>
       </c>
       <c r="K23" t="n">
-        <v>53.4</v>
+        <v>53.6</v>
       </c>
       <c r="L23" t="n">
-        <v>54.2</v>
+        <v>52.6</v>
       </c>
       <c r="M23" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1110&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1040&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>富邦-台北</t>
+          <t>國票-敦北法人</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.0212</v>
+        <v>0.0495</v>
       </c>
       <c r="D24" t="n">
-        <v>6977</v>
+        <v>22259</v>
       </c>
       <c r="E24" t="n">
-        <v>3645.8</v>
+        <v>-4117.9</v>
       </c>
       <c r="F24" t="n">
-        <v>3331.2</v>
+        <v>26377</v>
       </c>
       <c r="G24" t="n">
-        <v>-536</v>
+        <v>-6581</v>
       </c>
       <c r="H24" t="n">
-        <v>5491</v>
+        <v>2051</v>
       </c>
       <c r="I24" t="n">
-        <v>6028</v>
+        <v>8633</v>
       </c>
       <c r="J24" t="n">
-        <v>54.6</v>
+        <v>52.1</v>
       </c>
       <c r="K24" t="n">
-        <v>54.3</v>
+        <v>53.7</v>
       </c>
       <c r="L24" t="n">
-        <v>55</v>
+        <v>51.7</v>
       </c>
       <c r="M24" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9623&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=779c&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>元大-士林</t>
+          <t>美好-富順</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.0226</v>
+        <v>0.0221</v>
       </c>
       <c r="D25" t="n">
-        <v>6446.7</v>
+        <v>2152.5</v>
       </c>
       <c r="E25" t="n">
-        <v>12051.6</v>
+        <v>3031.7</v>
       </c>
       <c r="F25" t="n">
-        <v>-5604.8</v>
+        <v>-879.2</v>
       </c>
       <c r="G25" t="n">
-        <v>1877</v>
+        <v>171</v>
       </c>
       <c r="H25" t="n">
-        <v>5375</v>
+        <v>1814</v>
       </c>
       <c r="I25" t="n">
-        <v>3498</v>
+        <v>1642</v>
       </c>
       <c r="J25" t="n">
-        <v>53.1</v>
+        <v>53.7</v>
       </c>
       <c r="K25" t="n">
-        <v>51.7</v>
+        <v>52.8</v>
       </c>
       <c r="L25" t="n">
-        <v>55.2</v>
+        <v>54.7</v>
       </c>
       <c r="M25" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=981j&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=526K&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>凱基-信義</t>
+          <t>國票-安和</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1442</v>
+        <v>0.017</v>
       </c>
       <c r="D26" t="n">
-        <v>6308.6</v>
+        <v>1577.2</v>
       </c>
       <c r="E26" t="n">
-        <v>1712.1</v>
+        <v>1726.6</v>
       </c>
       <c r="F26" t="n">
-        <v>4596.5</v>
+        <v>-149.4</v>
       </c>
       <c r="G26" t="n">
-        <v>-433</v>
+        <v>38</v>
       </c>
       <c r="H26" t="n">
-        <v>324</v>
+        <v>1787</v>
       </c>
       <c r="I26" t="n">
-        <v>757</v>
+        <v>1748</v>
       </c>
       <c r="J26" t="n">
-        <v>57.8</v>
+        <v>52</v>
       </c>
       <c r="K26" t="n">
-        <v>54.1</v>
+        <v>51.5</v>
       </c>
       <c r="L26" t="n">
-        <v>59.4</v>
+        <v>52.5</v>
       </c>
       <c r="M26" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9216&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=779Z&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>凱基</t>
+          <t>兆豐-忠孝</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.0141</v>
+        <v>0.0306</v>
       </c>
       <c r="D27" t="n">
-        <v>6001.7</v>
+        <v>4415.7</v>
       </c>
       <c r="E27" t="n">
-        <v>3401.9</v>
+        <v>-1692.4</v>
       </c>
       <c r="F27" t="n">
-        <v>2599.8</v>
+        <v>6108.1</v>
       </c>
       <c r="G27" t="n">
-        <v>-535</v>
+        <v>-1081</v>
       </c>
       <c r="H27" t="n">
-        <v>7419</v>
+        <v>1600</v>
       </c>
       <c r="I27" t="n">
-        <v>7954</v>
+        <v>2682</v>
       </c>
       <c r="J27" t="n">
-        <v>53.4</v>
+        <v>53.7</v>
       </c>
       <c r="K27" t="n">
-        <v>53.2</v>
+        <v>54.4</v>
       </c>
       <c r="L27" t="n">
-        <v>53.6</v>
+        <v>53.3</v>
       </c>
       <c r="M27" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9200&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=700a&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>第一金-高雄</t>
+          <t>台灣企銀</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.061</v>
+        <v>0.0597</v>
       </c>
       <c r="D28" t="n">
-        <v>4292.1</v>
+        <v>8658.200000000001</v>
       </c>
       <c r="E28" t="n">
-        <v>486</v>
+        <v>1257.9</v>
       </c>
       <c r="F28" t="n">
-        <v>3806.1</v>
+        <v>7400.2</v>
       </c>
       <c r="G28" t="n">
-        <v>-516</v>
+        <v>-1138</v>
       </c>
       <c r="H28" t="n">
-        <v>744</v>
+        <v>1553</v>
       </c>
       <c r="I28" t="n">
-        <v>1260</v>
+        <v>2692</v>
       </c>
       <c r="J28" t="n">
-        <v>55.9</v>
+        <v>53.9</v>
       </c>
       <c r="K28" t="n">
-        <v>55.5</v>
+        <v>53.4</v>
       </c>
       <c r="L28" t="n">
-        <v>56.1</v>
+        <v>54.2</v>
       </c>
       <c r="M28" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=5383&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1110&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>元富-佳里</t>
+          <t>第一金-忠孝</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.0818</v>
+        <v>0.0232</v>
       </c>
       <c r="D29" t="n">
-        <v>3754.6</v>
+        <v>1635.7</v>
       </c>
       <c r="E29" t="n">
-        <v>1985.8</v>
+        <v>1687.9</v>
       </c>
       <c r="F29" t="n">
-        <v>1768.8</v>
+        <v>-52.2</v>
       </c>
       <c r="G29" t="n">
-        <v>-185</v>
+        <v>6</v>
       </c>
       <c r="H29" t="n">
-        <v>621</v>
+        <v>1265</v>
       </c>
       <c r="I29" t="n">
-        <v>806</v>
+        <v>1258</v>
       </c>
       <c r="J29" t="n">
-        <v>56.9</v>
+        <v>55.8</v>
       </c>
       <c r="K29" t="n">
-        <v>55.1</v>
+        <v>55.2</v>
       </c>
       <c r="L29" t="n">
-        <v>58.3</v>
+        <v>56.5</v>
       </c>
       <c r="M29" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=592w&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=538D&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>兆豐-忠孝</t>
+          <t>大和國泰</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.0228</v>
+        <v>0.0934</v>
       </c>
       <c r="D30" t="n">
-        <v>3279.6</v>
+        <v>41000</v>
       </c>
       <c r="E30" t="n">
-        <v>-1692.4</v>
+        <v>-3485.6</v>
       </c>
       <c r="F30" t="n">
-        <v>4972</v>
+        <v>44485.7</v>
       </c>
       <c r="G30" t="n">
-        <v>-1081</v>
+        <v>-6806</v>
       </c>
       <c r="H30" t="n">
-        <v>1600</v>
+        <v>1234</v>
       </c>
       <c r="I30" t="n">
-        <v>2682</v>
+        <v>8041</v>
       </c>
       <c r="J30" t="n">
-        <v>53.7</v>
+        <v>54.6</v>
       </c>
       <c r="K30" t="n">
-        <v>54.4</v>
+        <v>57.1</v>
       </c>
       <c r="L30" t="n">
-        <v>53.3</v>
+        <v>54.2</v>
       </c>
       <c r="M30" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=700a&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8890&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>元富</t>
+          <t>亞東</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0.004</v>
+        <v>0.03</v>
       </c>
       <c r="D31" t="n">
-        <v>3109.5</v>
+        <v>2215.5</v>
       </c>
       <c r="E31" t="n">
-        <v>-10938.1</v>
+        <v>1088</v>
       </c>
       <c r="F31" t="n">
-        <v>14047.6</v>
+        <v>1127.5</v>
       </c>
       <c r="G31" t="n">
-        <v>-2252</v>
+        <v>-141</v>
       </c>
       <c r="H31" t="n">
-        <v>11813</v>
+        <v>1196</v>
       </c>
       <c r="I31" t="n">
-        <v>14066</v>
+        <v>1337</v>
       </c>
       <c r="J31" t="n">
-        <v>55.4</v>
+        <v>55.3</v>
       </c>
       <c r="K31" t="n">
-        <v>55.9</v>
+        <v>54.8</v>
       </c>
       <c r="L31" t="n">
-        <v>55</v>
+        <v>55.7</v>
       </c>
       <c r="M31" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=5920&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=2180&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>彰銀-七賢</t>
+          <t>凱基-市政</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0.0765</v>
+        <v>0.033</v>
       </c>
       <c r="D32" t="n">
-        <v>3093.9</v>
+        <v>2703.4</v>
       </c>
       <c r="E32" t="n">
-        <v>877.6</v>
+        <v>392.2</v>
       </c>
       <c r="F32" t="n">
-        <v>2216.3</v>
+        <v>2311.2</v>
       </c>
       <c r="G32" t="n">
-        <v>-171</v>
+        <v>-242</v>
       </c>
       <c r="H32" t="n">
-        <v>492</v>
+        <v>1193</v>
       </c>
       <c r="I32" t="n">
-        <v>664</v>
+        <v>1436</v>
       </c>
       <c r="J32" t="n">
-        <v>60.9</v>
+        <v>57.1</v>
       </c>
       <c r="K32" t="n">
-        <v>59.9</v>
+        <v>56.9</v>
       </c>
       <c r="L32" t="n">
-        <v>61.6</v>
+        <v>57.2</v>
       </c>
       <c r="M32" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1232&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9239&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>中國信託-新竹</t>
+          <t>第一金</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>0.0608</v>
+        <v>0.0584</v>
       </c>
       <c r="D33" t="n">
-        <v>3084</v>
+        <v>12042.6</v>
       </c>
       <c r="E33" t="n">
-        <v>2053.1</v>
+        <v>-3129.4</v>
       </c>
       <c r="F33" t="n">
-        <v>1030.9</v>
+        <v>15172.1</v>
       </c>
       <c r="G33" t="n">
-        <v>-118</v>
+        <v>-2703</v>
       </c>
       <c r="H33" t="n">
-        <v>784</v>
+        <v>1122</v>
       </c>
       <c r="I33" t="n">
-        <v>902</v>
+        <v>3825</v>
       </c>
       <c r="J33" t="n">
-        <v>56.3</v>
+        <v>53.9</v>
       </c>
       <c r="K33" t="n">
-        <v>54.9</v>
+        <v>56.1</v>
       </c>
       <c r="L33" t="n">
-        <v>57.5</v>
+        <v>53.3</v>
       </c>
       <c r="M33" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=6165&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=5380&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>永豐金-古亭</t>
+          <t>元大-天母</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0.1096</v>
+        <v>0.0226</v>
       </c>
       <c r="D34" t="n">
-        <v>2878.8</v>
+        <v>1380.6</v>
       </c>
       <c r="E34" t="n">
-        <v>2914.8</v>
+        <v>2114.6</v>
       </c>
       <c r="F34" t="n">
-        <v>-36.1</v>
+        <v>-734</v>
       </c>
       <c r="G34" t="n">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="H34" t="n">
-        <v>460</v>
+        <v>1087</v>
       </c>
       <c r="I34" t="n">
-        <v>453</v>
+        <v>988</v>
       </c>
       <c r="J34" t="n">
-        <v>57.1</v>
+        <v>56.1</v>
       </c>
       <c r="K34" t="n">
-        <v>53.9</v>
+        <v>55.1</v>
       </c>
       <c r="L34" t="n">
-        <v>60.3</v>
+        <v>57.3</v>
       </c>
       <c r="M34" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9A9d&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=981I&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>凱基-市政</t>
+          <t>群益金鼎-館前</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>0.0299</v>
+        <v>0.0334</v>
       </c>
       <c r="D35" t="n">
-        <v>2448.2</v>
+        <v>3104.8</v>
       </c>
       <c r="E35" t="n">
-        <v>392.2</v>
+        <v>6.4</v>
       </c>
       <c r="F35" t="n">
-        <v>2056.1</v>
+        <v>3098.4</v>
       </c>
       <c r="G35" t="n">
-        <v>-242</v>
+        <v>-729</v>
       </c>
       <c r="H35" t="n">
-        <v>1193</v>
+        <v>1057</v>
       </c>
       <c r="I35" t="n">
-        <v>1436</v>
+        <v>1787</v>
       </c>
       <c r="J35" t="n">
-        <v>57.1</v>
+        <v>51.9</v>
       </c>
       <c r="K35" t="n">
-        <v>56.9</v>
+        <v>51.9</v>
       </c>
       <c r="L35" t="n">
-        <v>57.2</v>
+        <v>51.9</v>
       </c>
       <c r="M35" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9239&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=913Y&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>群益金鼎-館前</t>
+          <t>元大-文心</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.0252</v>
+        <v>0.0149</v>
       </c>
       <c r="D36" t="n">
-        <v>2338.3</v>
+        <v>774.7</v>
       </c>
       <c r="E36" t="n">
-        <v>6.4</v>
+        <v>-34.6</v>
       </c>
       <c r="F36" t="n">
-        <v>2331.9</v>
+        <v>809.4</v>
       </c>
       <c r="G36" t="n">
-        <v>-729</v>
+        <v>-155</v>
       </c>
       <c r="H36" t="n">
-        <v>1057</v>
+        <v>824</v>
       </c>
       <c r="I36" t="n">
-        <v>1787</v>
+        <v>980</v>
       </c>
       <c r="J36" t="n">
-        <v>51.9</v>
+        <v>52.9</v>
       </c>
       <c r="K36" t="n">
-        <v>51.9</v>
+        <v>52.9</v>
       </c>
       <c r="L36" t="n">
-        <v>51.9</v>
+        <v>52.9</v>
       </c>
       <c r="M36" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=913Y&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9868&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>美好-富順</t>
+          <t>彰銀</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.024</v>
+        <v>0.1153</v>
       </c>
       <c r="D37" t="n">
-        <v>2333.1</v>
+        <v>52197.9</v>
       </c>
       <c r="E37" t="n">
-        <v>3031.7</v>
+        <v>-1319.2</v>
       </c>
       <c r="F37" t="n">
-        <v>-698.6</v>
+        <v>53517.1</v>
       </c>
       <c r="G37" t="n">
-        <v>171</v>
+        <v>-7432</v>
       </c>
       <c r="H37" t="n">
-        <v>1814</v>
+        <v>790</v>
       </c>
       <c r="I37" t="n">
-        <v>1642</v>
+        <v>8222</v>
       </c>
       <c r="J37" t="n">
-        <v>53.7</v>
+        <v>55</v>
       </c>
       <c r="K37" t="n">
-        <v>52.8</v>
+        <v>56.6</v>
       </c>
       <c r="L37" t="n">
-        <v>54.7</v>
+        <v>54.9</v>
       </c>
       <c r="M37" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=526K&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1230&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>亞東</t>
+          <t>中國信託-新竹</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>0.028</v>
+        <v>0.06320000000000001</v>
       </c>
       <c r="D38" t="n">
-        <v>2067.4</v>
+        <v>3207.9</v>
       </c>
       <c r="E38" t="n">
-        <v>1088</v>
+        <v>2053.1</v>
       </c>
       <c r="F38" t="n">
-        <v>979.5</v>
+        <v>1154.8</v>
       </c>
       <c r="G38" t="n">
-        <v>-141</v>
+        <v>-118</v>
       </c>
       <c r="H38" t="n">
-        <v>1196</v>
+        <v>784</v>
       </c>
       <c r="I38" t="n">
-        <v>1337</v>
+        <v>902</v>
       </c>
       <c r="J38" t="n">
-        <v>55.3</v>
+        <v>56.3</v>
       </c>
       <c r="K38" t="n">
-        <v>54.8</v>
+        <v>54.9</v>
       </c>
       <c r="L38" t="n">
-        <v>55.7</v>
+        <v>57.5</v>
       </c>
       <c r="M38" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=2180&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=6165&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>國票-長城</t>
+          <t>土銀-高雄</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>0.0863</v>
+        <v>0.0255</v>
       </c>
       <c r="D39" t="n">
-        <v>1672.8</v>
+        <v>1252.4</v>
       </c>
       <c r="E39" t="n">
-        <v>714.8</v>
+        <v>401.7</v>
       </c>
       <c r="F39" t="n">
-        <v>958</v>
+        <v>850.7</v>
       </c>
       <c r="G39" t="n">
-        <v>-114</v>
+        <v>-128</v>
       </c>
       <c r="H39" t="n">
-        <v>232</v>
+        <v>778</v>
       </c>
       <c r="I39" t="n">
-        <v>347</v>
+        <v>907</v>
       </c>
       <c r="J39" t="n">
-        <v>55.8</v>
+        <v>54.1</v>
       </c>
       <c r="K39" t="n">
-        <v>54</v>
+        <v>53.8</v>
       </c>
       <c r="L39" t="n">
-        <v>57.1</v>
+        <v>54.3</v>
       </c>
       <c r="M39" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=779u&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1033&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>第一金-忠孝</t>
+          <t>第一金-高雄</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0.0233</v>
+        <v>0.0687</v>
       </c>
       <c r="D40" t="n">
-        <v>1643.1</v>
+        <v>4833.9</v>
       </c>
       <c r="E40" t="n">
-        <v>1687.9</v>
+        <v>486</v>
       </c>
       <c r="F40" t="n">
-        <v>-44.8</v>
+        <v>4347.9</v>
       </c>
       <c r="G40" t="n">
-        <v>6</v>
+        <v>-516</v>
       </c>
       <c r="H40" t="n">
-        <v>1265</v>
+        <v>744</v>
       </c>
       <c r="I40" t="n">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="J40" t="n">
-        <v>55.8</v>
+        <v>55.9</v>
       </c>
       <c r="K40" t="n">
-        <v>55.2</v>
+        <v>55.5</v>
       </c>
       <c r="L40" t="n">
-        <v>56.5</v>
+        <v>56.1</v>
       </c>
       <c r="M40" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=538D&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=5383&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>國票</t>
+          <t>元富-佳里</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.0076</v>
+        <v>0.0861</v>
       </c>
       <c r="D41" t="n">
-        <v>1635.3</v>
+        <v>3948.8</v>
       </c>
       <c r="E41" t="n">
-        <v>-123.7</v>
+        <v>1985.8</v>
       </c>
       <c r="F41" t="n">
-        <v>1759</v>
+        <v>1963.1</v>
       </c>
       <c r="G41" t="n">
-        <v>-228</v>
+        <v>-185</v>
       </c>
       <c r="H41" t="n">
-        <v>3581</v>
+        <v>621</v>
       </c>
       <c r="I41" t="n">
-        <v>3810</v>
+        <v>806</v>
       </c>
       <c r="J41" t="n">
-        <v>56.4</v>
+        <v>56.9</v>
       </c>
       <c r="K41" t="n">
-        <v>56.5</v>
+        <v>55.1</v>
       </c>
       <c r="L41" t="n">
-        <v>56.4</v>
+        <v>58.3</v>
       </c>
       <c r="M41" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=7790&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=592w&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>國票-安和</t>
+          <t>華南永昌-嘉義</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.0174</v>
+        <v>0.0677</v>
       </c>
       <c r="D42" t="n">
-        <v>1618.1</v>
+        <v>10728.2</v>
       </c>
       <c r="E42" t="n">
-        <v>1726.6</v>
+        <v>-2227.5</v>
       </c>
       <c r="F42" t="n">
-        <v>-108.4</v>
+        <v>12955.7</v>
       </c>
       <c r="G42" t="n">
-        <v>38</v>
+        <v>-2357</v>
       </c>
       <c r="H42" t="n">
-        <v>1787</v>
+        <v>587</v>
       </c>
       <c r="I42" t="n">
-        <v>1748</v>
+        <v>2945</v>
       </c>
       <c r="J42" t="n">
-        <v>52</v>
+        <v>53.8</v>
       </c>
       <c r="K42" t="n">
-        <v>51.5</v>
+        <v>57</v>
       </c>
       <c r="L42" t="n">
-        <v>52.5</v>
+        <v>53.2</v>
       </c>
       <c r="M42" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=779Z&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9314&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>元大-天母</t>
+          <t>群益金鼎-萬華</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.0243</v>
+        <v>0.0296</v>
       </c>
       <c r="D43" t="n">
-        <v>1484.6</v>
+        <v>917.9</v>
       </c>
       <c r="E43" t="n">
-        <v>2114.6</v>
+        <v>1252.8</v>
       </c>
       <c r="F43" t="n">
-        <v>-630.1</v>
+        <v>-334.8</v>
       </c>
       <c r="G43" t="n">
-        <v>98</v>
+        <v>43</v>
       </c>
       <c r="H43" t="n">
-        <v>1087</v>
+        <v>548</v>
       </c>
       <c r="I43" t="n">
-        <v>988</v>
+        <v>505</v>
       </c>
       <c r="J43" t="n">
-        <v>56.1</v>
+        <v>56.7</v>
       </c>
       <c r="K43" t="n">
-        <v>55.1</v>
+        <v>55.5</v>
       </c>
       <c r="L43" t="n">
-        <v>57.3</v>
+        <v>58</v>
       </c>
       <c r="M43" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=981I&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=913I&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>群益金鼎-內湖</t>
+          <t>彰銀-七賢</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0.0334</v>
+        <v>0.081</v>
       </c>
       <c r="D44" t="n">
-        <v>1371.8</v>
+        <v>3274.5</v>
       </c>
       <c r="E44" t="n">
-        <v>-607</v>
+        <v>877.6</v>
       </c>
       <c r="F44" t="n">
-        <v>1978.8</v>
+        <v>2396.9</v>
       </c>
       <c r="G44" t="n">
-        <v>-294</v>
+        <v>-171</v>
       </c>
       <c r="H44" t="n">
-        <v>438</v>
+        <v>492</v>
       </c>
       <c r="I44" t="n">
-        <v>733</v>
+        <v>664</v>
       </c>
       <c r="J44" t="n">
-        <v>56</v>
+        <v>60.9</v>
       </c>
       <c r="K44" t="n">
-        <v>56.8</v>
+        <v>59.9</v>
       </c>
       <c r="L44" t="n">
-        <v>55.5</v>
+        <v>61.6</v>
       </c>
       <c r="M44" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=918d&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1232&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>康和-澎湖</t>
+          <t>永豐金-古亭</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.08550000000000001</v>
+        <v>0.1093</v>
       </c>
       <c r="D45" t="n">
-        <v>1253.2</v>
+        <v>2871.4</v>
       </c>
       <c r="E45" t="n">
-        <v>552.5</v>
+        <v>2914.8</v>
       </c>
       <c r="F45" t="n">
-        <v>700.7</v>
+        <v>-43.4</v>
       </c>
       <c r="G45" t="n">
-        <v>-67</v>
+        <v>6</v>
       </c>
       <c r="H45" t="n">
-        <v>186</v>
+        <v>460</v>
       </c>
       <c r="I45" t="n">
-        <v>253</v>
+        <v>453</v>
       </c>
       <c r="J45" t="n">
-        <v>58</v>
+        <v>57.1</v>
       </c>
       <c r="K45" t="n">
-        <v>56.2</v>
+        <v>53.9</v>
       </c>
       <c r="L45" t="n">
-        <v>59.2</v>
+        <v>60.3</v>
       </c>
       <c r="M45" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=845E&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9A9d&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>京城</t>
+          <t>群益金鼎-內湖</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.06559999999999999</v>
+        <v>0.04099999999999999</v>
       </c>
       <c r="D46" t="n">
-        <v>1160.8</v>
+        <v>1681.6</v>
       </c>
       <c r="E46" t="n">
-        <v>1308.5</v>
+        <v>-607</v>
       </c>
       <c r="F46" t="n">
-        <v>-147.7</v>
+        <v>2288.5</v>
       </c>
       <c r="G46" t="n">
-        <v>72</v>
+        <v>-294</v>
       </c>
       <c r="H46" t="n">
-        <v>334</v>
+        <v>438</v>
       </c>
       <c r="I46" t="n">
-        <v>262</v>
+        <v>733</v>
       </c>
       <c r="J46" t="n">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K46" t="n">
-        <v>50.8</v>
+        <v>56.8</v>
       </c>
       <c r="L46" t="n">
-        <v>55.8</v>
+        <v>55.5</v>
       </c>
       <c r="M46" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=8490&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=918d&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>土銀-高雄</t>
+          <t>土銀-台中</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.0228</v>
+        <v>0.0363</v>
       </c>
       <c r="D47" t="n">
-        <v>1116.9</v>
+        <v>810.8</v>
       </c>
       <c r="E47" t="n">
-        <v>401.7</v>
+        <v>541.2</v>
       </c>
       <c r="F47" t="n">
-        <v>715.2</v>
+        <v>269.6</v>
       </c>
       <c r="G47" t="n">
-        <v>-128</v>
+        <v>-31</v>
       </c>
       <c r="H47" t="n">
-        <v>778</v>
+        <v>371</v>
       </c>
       <c r="I47" t="n">
-        <v>907</v>
+        <v>403</v>
       </c>
       <c r="J47" t="n">
-        <v>54.1</v>
+        <v>55.4</v>
       </c>
       <c r="K47" t="n">
-        <v>53.8</v>
+        <v>54.7</v>
       </c>
       <c r="L47" t="n">
-        <v>54.3</v>
+        <v>56.1</v>
       </c>
       <c r="M47" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1033&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=1031&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>群益金鼎-萬華</t>
+          <t>京城</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0.031</v>
+        <v>0.0613</v>
       </c>
       <c r="D48" t="n">
-        <v>963.1</v>
+        <v>1085.2</v>
       </c>
       <c r="E48" t="n">
-        <v>1252.8</v>
+        <v>1308.5</v>
       </c>
       <c r="F48" t="n">
-        <v>-289.7</v>
+        <v>-223.3</v>
       </c>
       <c r="G48" t="n">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="H48" t="n">
-        <v>548</v>
+        <v>334</v>
       </c>
       <c r="I48" t="n">
-        <v>505</v>
+        <v>262</v>
       </c>
       <c r="J48" t="n">
-        <v>56.7</v>
+        <v>53</v>
       </c>
       <c r="K48" t="n">
-        <v>55.5</v>
+        <v>50.8</v>
       </c>
       <c r="L48" t="n">
-        <v>58</v>
+        <v>55.8</v>
       </c>
       <c r="M48" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=913I&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=8490&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>土銀-台中</t>
+          <t>凱基-信義</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0.0348</v>
+        <v>0.1546</v>
       </c>
       <c r="D49" t="n">
-        <v>777.2</v>
+        <v>6763.3</v>
       </c>
       <c r="E49" t="n">
-        <v>541.2</v>
+        <v>1712.1</v>
       </c>
       <c r="F49" t="n">
-        <v>236</v>
+        <v>5051.2</v>
       </c>
       <c r="G49" t="n">
-        <v>-31</v>
+        <v>-433</v>
       </c>
       <c r="H49" t="n">
-        <v>371</v>
+        <v>324</v>
       </c>
       <c r="I49" t="n">
-        <v>403</v>
+        <v>757</v>
       </c>
       <c r="J49" t="n">
-        <v>55.4</v>
+        <v>57.8</v>
       </c>
       <c r="K49" t="n">
-        <v>54.7</v>
+        <v>54.1</v>
       </c>
       <c r="L49" t="n">
-        <v>56.1</v>
+        <v>59.4</v>
       </c>
       <c r="M49" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=1031&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=9216&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>華南永昌</t>
+          <t>國票-長城</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0.0019</v>
+        <v>0.0926</v>
       </c>
       <c r="D50" t="n">
-        <v>716.7</v>
+        <v>1793.6</v>
       </c>
       <c r="E50" t="n">
-        <v>385.2</v>
+        <v>714.8</v>
       </c>
       <c r="F50" t="n">
-        <v>331.5</v>
+        <v>1078.8</v>
       </c>
       <c r="G50" t="n">
-        <v>-55</v>
+        <v>-114</v>
       </c>
       <c r="H50" t="n">
-        <v>6797</v>
+        <v>232</v>
       </c>
       <c r="I50" t="n">
-        <v>6853</v>
+        <v>347</v>
       </c>
       <c r="J50" t="n">
-        <v>54.6</v>
+        <v>55.8</v>
       </c>
       <c r="K50" t="n">
-        <v>54.6</v>
+        <v>54</v>
       </c>
       <c r="L50" t="n">
-        <v>54.7</v>
+        <v>57.1</v>
       </c>
       <c r="M50" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=9300&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=779u&amp;no=1301</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>寶盛</t>
+          <t>康和-澎湖</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.1215</v>
+        <v>0.09029999999999999</v>
       </c>
       <c r="D51" t="n">
-        <v>707.2</v>
+        <v>1323.5</v>
       </c>
       <c r="E51" t="n">
-        <v>657.8</v>
+        <v>552.5</v>
       </c>
       <c r="F51" t="n">
-        <v>49.4</v>
+        <v>771.1</v>
       </c>
       <c r="G51" t="n">
-        <v>-4</v>
+        <v>-67</v>
       </c>
       <c r="H51" t="n">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="I51" t="n">
-        <v>105</v>
+        <v>253</v>
       </c>
       <c r="J51" t="n">
-        <v>55.4</v>
+        <v>58</v>
       </c>
       <c r="K51" t="n">
-        <v>52.1</v>
+        <v>56.2</v>
       </c>
       <c r="L51" t="n">
-        <v>58.6</v>
+        <v>59.2</v>
       </c>
       <c r="M51" t="n">
-        <v>48.8</v>
+        <v>47.7</v>
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>/stock/brokertrace.aspx?bno=5460&amp;no=1301</t>
+          <t>/stock/brokertrace.aspx?bno=845E&amp;no=1301</t>
         </is>
       </c>
     </row>

</xml_diff>